<commit_message>
work on fuzzy string match and comparing samples
</commit_message>
<xml_diff>
--- a/data/samples/sample_museum_search_with_loc.xlsx
+++ b/data/samples/sample_museum_search_with_loc.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="153">
   <si>
     <t>google_rank</t>
   </si>
@@ -447,12 +447,39 @@
   <si>
     <t>no_resource</t>
   </si>
+  <si>
+    <t>correct_url</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/NorthLanHeritage/</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/ThomasCarlylesBirthplaceNTS/</t>
+  </si>
+  <si>
+    <t>https://twitter.com/thenmmuk?lang=en</t>
+  </si>
+  <si>
+    <t>https://twitter.com/museumofflight?lang=en</t>
+  </si>
+  <si>
+    <t>https://twitter.com/nvmuk</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>facebook</t>
+  </si>
+  <si>
+    <t>twitter</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -479,6 +506,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -535,7 +568,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -549,6 +582,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -851,1078 +887,1398 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3749"/>
+  <dimension ref="A1:I3749"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="G45" sqref="G45"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H61" sqref="H61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.5703125" customWidth="1"/>
-    <col min="2" max="2" width="39.28515625" customWidth="1"/>
-    <col min="3" max="3" width="87.5703125" customWidth="1"/>
-    <col min="4" max="6" width="37.28515625" customWidth="1"/>
-    <col min="7" max="7" width="23.5703125" customWidth="1"/>
+    <col min="2" max="3" width="39.28515625" customWidth="1"/>
+    <col min="4" max="4" width="54.85546875" customWidth="1"/>
+    <col min="5" max="5" width="21.42578125" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="37.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="F1" s="7" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="I1" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
         <v>44</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" t="b">
+      <c r="F2" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
+      <c r="I2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="b">
+      <c r="F3" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="I3" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D4" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="b">
+      <c r="F4" t="b">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>141</v>
       </c>
-      <c r="G4" t="b">
+      <c r="H4" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7">
+      <c r="I4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" t="b">
+      <c r="F5" t="b">
         <v>0</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>141</v>
       </c>
-      <c r="G5" t="b">
+      <c r="H5" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:7">
+      <c r="I5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>49</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>14</v>
       </c>
-      <c r="E6" t="b">
+      <c r="F6" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:7">
+      <c r="I6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
         <v>50</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" t="b">
+      <c r="F7" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7">
+      <c r="I7" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
         <v>52</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="b">
+      <c r="F8" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:7">
+      <c r="I8" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s">
         <v>54</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="b">
+      <c r="F9" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:7">
+      <c r="I9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s">
         <v>56</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="b">
+      <c r="F10" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:7">
+      <c r="I10" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>1</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11" t="s">
         <v>58</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="b">
+      <c r="F11" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:7">
+      <c r="I11" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" t="s">
         <v>59</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>24</v>
       </c>
-      <c r="E12" t="b">
+      <c r="F12" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:7">
+      <c r="I12" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" t="s">
         <v>61</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>26</v>
       </c>
-      <c r="E13" t="b">
+      <c r="F13" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:7">
+      <c r="I13" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" t="s">
         <v>63</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>27</v>
       </c>
-      <c r="E14" t="b">
+      <c r="F14" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:7">
+      <c r="I14" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>1</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" t="s">
         <v>65</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>28</v>
       </c>
-      <c r="E15" t="b">
+      <c r="F15" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:7">
+      <c r="I15" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>1</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" t="s">
         <v>67</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>29</v>
       </c>
-      <c r="E16" t="b">
+      <c r="F16" t="b">
         <v>0</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>141</v>
       </c>
-      <c r="G16" t="b">
+      <c r="H16" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:7">
+      <c r="I16" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
         <v>68</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>30</v>
       </c>
-      <c r="E17" t="b">
+      <c r="F17" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:7">
+      <c r="I17" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D18" t="s">
         <v>70</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>32</v>
       </c>
-      <c r="E18" t="b">
+      <c r="F18" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:7">
+      <c r="I18" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
         <v>71</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>33</v>
       </c>
-      <c r="E19" t="b">
+      <c r="F19" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:7">
+      <c r="I19" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D20" t="s">
         <v>73</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>35</v>
       </c>
-      <c r="E20" t="b">
+      <c r="F20" t="b">
         <v>0</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="I20" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D21" t="s">
         <v>75</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>36</v>
       </c>
-      <c r="E21" t="b">
+      <c r="F21" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:7">
+      <c r="I21" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" t="s">
         <v>77</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>37</v>
       </c>
-      <c r="E22" t="b">
+      <c r="F22" t="b">
         <v>0</v>
       </c>
-      <c r="F22" t="s">
+      <c r="G22" t="s">
         <v>141</v>
       </c>
-      <c r="G22" t="b">
+      <c r="H22" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:7">
+      <c r="I22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
         <v>79</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>39</v>
       </c>
-      <c r="E23" t="b">
+      <c r="F23" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:7">
+      <c r="I23" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9">
       <c r="A24">
         <v>1</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D24" t="s">
         <v>81</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>40</v>
       </c>
-      <c r="E24" t="b">
+      <c r="F24" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:7">
+      <c r="I24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9">
       <c r="A25">
         <v>1</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D25" t="s">
         <v>83</v>
       </c>
-      <c r="D25" t="s">
+      <c r="E25" t="s">
         <v>41</v>
       </c>
-      <c r="E25" t="b">
+      <c r="F25" t="b">
         <v>1</v>
       </c>
-      <c r="F25" t="s">
+      <c r="G25" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="26" spans="1:7">
+      <c r="I25" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D26" t="s">
         <v>85</v>
       </c>
-      <c r="D26" t="s">
+      <c r="E26" t="s">
         <v>42</v>
       </c>
-      <c r="E26" t="b">
+      <c r="F26" t="b">
         <v>0</v>
       </c>
-      <c r="F26" t="s">
+      <c r="G26" t="s">
         <v>141</v>
       </c>
-      <c r="G26" t="b">
+      <c r="H26" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:7">
+      <c r="I26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9">
       <c r="A27">
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="D27" t="s">
         <v>87</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>43</v>
       </c>
-      <c r="E27" t="b">
+      <c r="F27" t="b">
         <v>0</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="28" spans="1:7">
+      <c r="I27" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9">
       <c r="A28">
         <v>1</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" t="s">
         <v>88</v>
       </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>4</v>
       </c>
-      <c r="E28" t="b">
+      <c r="F28" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:7">
+      <c r="I28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9">
       <c r="A29">
         <v>1</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" t="s">
         <v>89</v>
       </c>
-      <c r="D29" t="s">
+      <c r="E29" t="s">
         <v>7</v>
       </c>
-      <c r="E29" t="b">
+      <c r="F29" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:7">
+      <c r="I29" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D30" t="s">
         <v>91</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>10</v>
       </c>
-      <c r="E30" t="b">
+      <c r="F30" t="b">
         <v>0</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>141</v>
       </c>
-      <c r="G30" t="b">
+      <c r="H30" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:7">
+      <c r="I30" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D31" t="s">
         <v>92</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>12</v>
       </c>
-      <c r="E31" t="b">
+      <c r="F31" t="b">
         <v>0</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>141</v>
       </c>
-      <c r="G31" t="b">
+      <c r="H31" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:7">
+      <c r="I31" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D32" t="s">
         <v>93</v>
       </c>
-      <c r="D32" t="s">
+      <c r="E32" t="s">
         <v>14</v>
       </c>
-      <c r="E32" t="b">
+      <c r="F32" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:7">
+      <c r="I32" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9">
       <c r="A33">
         <v>1</v>
       </c>
       <c r="B33" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D33" t="s">
         <v>94</v>
       </c>
-      <c r="D33" t="s">
+      <c r="E33" t="s">
         <v>17</v>
       </c>
-      <c r="E33" t="b">
+      <c r="F33" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
+      <c r="I33" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9">
       <c r="A34">
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D34" t="s">
         <v>96</v>
       </c>
-      <c r="D34" t="s">
+      <c r="E34" t="s">
         <v>20</v>
       </c>
-      <c r="E34" t="b">
+      <c r="F34" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:7">
+      <c r="I34" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9">
       <c r="A35">
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D35" t="s">
         <v>98</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>21</v>
       </c>
-      <c r="E35" t="b">
+      <c r="F35" t="b">
         <v>0</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>141</v>
       </c>
-      <c r="G35" t="b">
+      <c r="H35" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:7">
+      <c r="I35" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9">
       <c r="A36">
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D36" t="s">
         <v>100</v>
       </c>
-      <c r="D36" t="s">
+      <c r="E36" t="s">
         <v>22</v>
       </c>
-      <c r="E36" t="b">
+      <c r="F36" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:7">
+      <c r="I36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
       <c r="A37">
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D37" t="s">
         <v>102</v>
       </c>
-      <c r="D37" t="s">
+      <c r="E37" t="s">
         <v>23</v>
       </c>
-      <c r="E37" t="b">
+      <c r="F37" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="38" spans="1:7">
+      <c r="I37" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
       <c r="A38">
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D38" t="s">
         <v>104</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>24</v>
       </c>
-      <c r="E38" t="b">
+      <c r="F38" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:7">
+      <c r="I38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
       <c r="A39">
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" t="s">
         <v>106</v>
       </c>
-      <c r="D39" t="s">
+      <c r="E39" t="s">
         <v>26</v>
       </c>
-      <c r="E39" t="b">
+      <c r="F39" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="I39" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
       <c r="A40">
         <v>1</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D40" t="s">
         <v>108</v>
       </c>
-      <c r="D40" t="s">
+      <c r="E40" t="s">
         <v>27</v>
       </c>
-      <c r="E40" t="b">
+      <c r="F40" t="b">
         <v>0</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>141</v>
       </c>
-      <c r="G40" t="b">
+      <c r="H40" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:7">
+      <c r="I40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
       <c r="A41">
         <v>1</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" t="s">
         <v>110</v>
       </c>
-      <c r="D41" t="s">
+      <c r="E41" t="s">
         <v>28</v>
       </c>
-      <c r="E41" t="b">
+      <c r="F41" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="42" spans="1:7">
+      <c r="I41" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
       <c r="A42">
         <v>1</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D42" t="s">
         <v>112</v>
       </c>
-      <c r="D42" t="s">
+      <c r="E42" t="s">
         <v>29</v>
       </c>
-      <c r="E42" t="b">
+      <c r="F42" t="b">
         <v>0</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>141</v>
       </c>
-      <c r="G42" t="b">
+      <c r="H42" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:7">
+      <c r="I42" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
       <c r="A43">
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D43" t="s">
         <v>114</v>
       </c>
-      <c r="D43" t="s">
+      <c r="E43" t="s">
         <v>30</v>
       </c>
-      <c r="E43" t="b">
+      <c r="F43" t="b">
         <v>0</v>
       </c>
-      <c r="F43" t="s">
+      <c r="G43" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="44" spans="1:7">
+      <c r="I43" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
       <c r="A44">
         <v>1</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="D44" t="s">
         <v>116</v>
       </c>
-      <c r="D44" t="s">
+      <c r="E44" t="s">
         <v>32</v>
       </c>
-      <c r="E44" t="b">
+      <c r="F44" t="b">
         <v>0</v>
       </c>
-      <c r="F44" t="s">
+      <c r="G44" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="45" spans="1:7">
+      <c r="I44" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
       <c r="A45">
         <v>1</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D45" t="s">
         <v>118</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>33</v>
       </c>
-      <c r="E45" t="b">
+      <c r="F45" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="46" spans="1:7">
+      <c r="I45" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
       <c r="A46">
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D46" t="s">
         <v>120</v>
       </c>
-      <c r="D46" t="s">
+      <c r="E46" t="s">
         <v>35</v>
       </c>
-      <c r="E46" t="b">
+      <c r="F46" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:7">
+      <c r="I46" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
       <c r="A47">
         <v>1</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="D47" t="s">
         <v>122</v>
       </c>
-      <c r="D47" t="s">
+      <c r="E47" t="s">
         <v>36</v>
       </c>
-      <c r="E47" t="b">
+      <c r="F47" t="b">
         <v>1</v>
       </c>
-      <c r="F47" t="s">
+      <c r="G47" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="48" spans="1:7">
+      <c r="I47" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
       <c r="A48">
         <v>1</v>
       </c>
       <c r="B48" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D48" t="s">
         <v>123</v>
       </c>
-      <c r="D48" t="s">
+      <c r="E48" t="s">
         <v>37</v>
       </c>
-      <c r="E48" t="b">
+      <c r="F48" t="b">
         <v>0</v>
       </c>
-      <c r="F48" t="s">
+      <c r="G48" t="s">
         <v>141</v>
       </c>
-      <c r="G48" t="b">
+      <c r="H48" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:7">
+      <c r="I48" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>1</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D49" t="s">
         <v>125</v>
       </c>
-      <c r="D49" t="s">
+      <c r="E49" t="s">
         <v>39</v>
       </c>
-      <c r="E49" t="b">
+      <c r="F49" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="50" spans="1:7">
+      <c r="I49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>1</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D50" t="s">
         <v>127</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>40</v>
       </c>
-      <c r="E50" t="b">
+      <c r="F50" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:7">
+      <c r="I50" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>1</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" t="s">
         <v>129</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>41</v>
       </c>
-      <c r="E51" t="b">
+      <c r="F51" t="b">
         <v>0</v>
       </c>
-      <c r="F51" t="s">
+      <c r="G51" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="52" spans="1:7">
+      <c r="I51" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9">
       <c r="A52">
         <v>1</v>
       </c>
       <c r="B52" s="3" t="s">
         <v>130</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D52" t="s">
         <v>131</v>
       </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>42</v>
       </c>
-      <c r="E52" t="b">
+      <c r="F52" t="b">
         <v>0</v>
       </c>
-      <c r="F52" t="s">
+      <c r="G52" t="s">
         <v>141</v>
       </c>
-      <c r="G52" t="b">
+      <c r="H52" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:7">
+      <c r="I52" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9">
       <c r="A53">
         <v>1</v>
       </c>
       <c r="B53" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="D53" t="s">
         <v>133</v>
       </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>43</v>
       </c>
-      <c r="E53" t="b">
+      <c r="F53" t="b">
         <v>0</v>
       </c>
-      <c r="F53" t="s">
+      <c r="G53" t="s">
         <v>141</v>
       </c>
-      <c r="G53" t="b">
+      <c r="H53" t="b">
         <v>1</v>
       </c>
-    </row>
-    <row r="54" spans="1:7">
+      <c r="I53" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9">
       <c r="A54">
         <v>2</v>
       </c>
     </row>
-    <row r="55" spans="1:7">
+    <row r="55" spans="1:9">
       <c r="A55">
         <v>2</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:9">
       <c r="A56">
         <v>2</v>
       </c>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:9">
       <c r="A57">
         <v>2</v>
       </c>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:9">
       <c r="A58">
         <v>2</v>
       </c>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:9">
       <c r="A59">
         <v>2</v>
       </c>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:9">
       <c r="A60">
         <v>2</v>
       </c>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:9">
       <c r="A61">
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:9">
       <c r="A62">
         <v>2</v>
       </c>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:9">
       <c r="A63">
         <v>2</v>
       </c>
     </row>
-    <row r="64" spans="1:7">
+    <row r="64" spans="1:9">
       <c r="A64">
         <v>2</v>
       </c>
@@ -20407,8 +20763,40 @@
     <hyperlink ref="B25" r:id="rId48"/>
     <hyperlink ref="B26" r:id="rId49"/>
     <hyperlink ref="B27" r:id="rId50"/>
+    <hyperlink ref="C2" r:id="rId51"/>
+    <hyperlink ref="C3" r:id="rId52"/>
+    <hyperlink ref="C6" r:id="rId53"/>
+    <hyperlink ref="C7" r:id="rId54"/>
+    <hyperlink ref="C8" r:id="rId55"/>
+    <hyperlink ref="C9" r:id="rId56"/>
+    <hyperlink ref="C10" r:id="rId57"/>
+    <hyperlink ref="C11" r:id="rId58"/>
+    <hyperlink ref="C12" r:id="rId59"/>
+    <hyperlink ref="C13" r:id="rId60"/>
+    <hyperlink ref="C14" r:id="rId61"/>
+    <hyperlink ref="C15" r:id="rId62"/>
+    <hyperlink ref="C17" r:id="rId63"/>
+    <hyperlink ref="C18" r:id="rId64"/>
+    <hyperlink ref="C19" r:id="rId65"/>
+    <hyperlink ref="C21" r:id="rId66"/>
+    <hyperlink ref="C23" r:id="rId67"/>
+    <hyperlink ref="C24" r:id="rId68"/>
+    <hyperlink ref="C25" r:id="rId69"/>
+    <hyperlink ref="C28" r:id="rId70"/>
+    <hyperlink ref="C29" r:id="rId71"/>
+    <hyperlink ref="C34" r:id="rId72"/>
+    <hyperlink ref="C36" r:id="rId73"/>
+    <hyperlink ref="C37" r:id="rId74"/>
+    <hyperlink ref="C38" r:id="rId75"/>
+    <hyperlink ref="C39" r:id="rId76"/>
+    <hyperlink ref="C41" r:id="rId77"/>
+    <hyperlink ref="C45" r:id="rId78"/>
+    <hyperlink ref="C46" r:id="rId79"/>
+    <hyperlink ref="C47" r:id="rId80"/>
+    <hyperlink ref="C49" r:id="rId81"/>
+    <hyperlink ref="C50" r:id="rId82"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId51"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId83"/>
 </worksheet>
 </file>
</xml_diff>